<commit_message>
update form dan data
</commit_message>
<xml_diff>
--- a/public/form/Form-input-data-kendaraan.xlsx
+++ b/public/form/Form-input-data-kendaraan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\PHP\antikendor\public\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CF7420-39ED-4450-A431-6F749203CB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15B5CDF-3B71-4939-8E6D-AC6950353282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AA5CEDE7-6150-4FD0-80D3-5900678BA5FB}"/>
   </bookViews>
@@ -35,8 +35,138 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ismail - [2010]</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{8BA2D8BD-AB51-4261-9DC8-FBFE87E795FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ismail - [2010]:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bisa dikosongi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{719257A8-64D7-42CD-95EC-020FD11E75C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ismail - [2010]:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bisa dikosongi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{B46CBF76-65AE-45B4-9A66-D0C7D41B2EAA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ismail - [2010]:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bisa dikosongi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{CCEA49ED-7806-49DD-8548-004A3A29C353}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ismail - [2010]:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bisa dikosongi.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{C62839A3-8203-47CE-B3A4-F2F35DBDD3DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ismail - [2010]:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bisa dikosongi.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Nomor Polisi</t>
   </si>
@@ -98,7 +228,10 @@
     <t>CONTOH</t>
   </si>
   <si>
-    <t>JANGAN DIHAPUS</t>
+    <t>085157626557</t>
+  </si>
+  <si>
+    <t>------ BARIS INI JANGAN DIHAPUS ------</t>
   </si>
 </sst>
 </file>
@@ -108,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="42" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,7 +259,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,13 +287,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +309,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,36 +369,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,9 +381,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,6 +392,34 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -627,19 +786,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D8FCF2-63FB-4B6F-9D7E-B68EF406A33D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D8FCF2-63FB-4B6F-9D7E-B68EF406A33D}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68" style="2" bestFit="1" customWidth="1"/>
@@ -650,92 +809,94 @@
     <col min="9" max="9" width="17.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12">
+      <c r="J2" s="24">
         <v>3399600</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="24">
         <v>101000</v>
       </c>
-      <c r="L2" s="22">
+      <c r="L2" s="25">
         <v>43840</v>
       </c>
-      <c r="M2" s="22">
+      <c r="M2" s="25">
         <v>43840</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
@@ -748,11 +909,11 @@
       <c r="I3" s="7"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="24"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
@@ -765,11 +926,11 @@
       <c r="I4" s="7"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
@@ -782,8 +943,8 @@
       <c r="I5" s="7"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
@@ -799,5 +960,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>